<commit_message>
Actualización de casos de Prueba
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -433,13 +433,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -955,7 +955,7 @@
         <v>70</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,7 +969,7 @@
         <v>72</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>